<commit_message>
“Laboratorio 7 – Entrega pre-final”
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
+++ b/Docs/ISIS1225 - Tablas de Datos Lab 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/2022-20/Laboratorios/Lab 07 - Colisiones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Documents\Uniandes\Segundo Semestre\EDA\Laboratorio 7\LabCollision-S07-G09\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="726" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F54888-DFB5-49D6-8E23-12D138256747}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEF53C4-CB77-4EDA-BB75-D283DA52D577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="887" windowWidth="2273" windowHeight="1493" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <r>
       <t>Factor de Carga</t>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Tiempo de Ejecución Real @SC [ms]</t>
+  </si>
+  <si>
+    <t>Columna1</t>
   </si>
 </sst>
 </file>
@@ -144,75 +147,78 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -230,14 +236,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -256,7 +261,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -290,6 +294,24 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -316,6 +338,70 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -366,6 +452,66 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -392,6 +538,46 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -442,6 +628,22 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -459,7 +661,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -532,7 +734,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -619,7 +821,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -631,16 +833,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>36090.023000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>35684.266799999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>35653.134399999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>35636.795399999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,16 +854,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>1631.7757999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>1552.0115999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>1395.5350000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>1500.5300000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -750,7 +952,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -762,13 +964,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>35696.243200000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>35644.337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35639.712000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>35637.130799999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -780,13 +985,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>105</c:v>
+                  <c:v>1579.0524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125</c:v>
+                  <c:v>1587.9334000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1560.2134000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>1600.577</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -881,7 +1089,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -919,7 +1127,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1087681551"/>
@@ -1006,7 +1214,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1044,7 +1252,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1087686127"/>
@@ -1086,7 +1294,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1116,7 +1324,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1125,7 +1333,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1189,7 +1397,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1313,7 +1521,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1346,16 +1554,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>36090.023000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>35684.266799999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>35653.134399999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>35636.795399999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1471,7 +1679,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1504,13 +1712,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>35696.243200000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>35644.337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35639.712000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>35637.130799999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1600,7 +1811,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1635,7 +1846,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1086959919"/>
@@ -1708,7 +1919,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1742,7 +1953,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1086958255"/>
@@ -1781,7 +1992,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1811,7 +2022,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2890,7 +3101,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CAFD5B44-21B9-42C7-B503-C146EF1BA3EE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="63" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2901,7 +3112,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{680E7371-595A-4F03-ABE3-E0257A96E5F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="63" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2912,7 +3123,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="9293175" cy="6067778"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2945,7 +3156,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9293175" cy="6067778"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2975,31 +3186,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:C6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)"/>
-    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:D6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D6" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{F280BCD9-1105-4F25-860B-4E27D28E75B2}" name="Consumo de Datos [kB]" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Tiempo de Ejecución Real @LP [ms]" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C071496D-ECC6-4563-BDF8-FF1D6E09F743}" name="Columna1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:C14" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A10:C14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A10:D14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A10:D14" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{89028F05-533D-401C-8D1A-1C8737D88894}" name="Consumo de Datos [kB]" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Tiempo de Ejecución Real @SC [ms]" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{440BAEAA-2EF8-4B89-B638-2691D279DCC9}" name="Columna1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3295,150 +3508,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C14"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.64453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3" s="10">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>0.1</v>
       </c>
       <c r="B3" s="5">
-        <v>100</v>
+        <f>36090.023</f>
+        <v>36090.023000000001</v>
       </c>
-      <c r="C3" s="8">
-        <v>75</v>
+      <c r="C3" s="6">
+        <f>AVERAGE(1625.791,1650.989,1642.987,1596.712,1642.4)</f>
+        <v>1631.7757999999999</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="B4" s="8">
+        <f>AVERAGE(35684.234,35684.234,35684.562,35684.234,35684.07)</f>
+        <v>35684.266799999998</v>
+      </c>
+      <c r="C4" s="6">
+        <f>AVERAGE(1546.889,1666.32,1428.832,1582.85,1535.167 )</f>
+        <v>1552.0115999999998</v>
+      </c>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="B5" s="8">
+        <f>AVERAGE(35657.531,35656.875,35637.024,35657.039,35657.203)</f>
+        <v>35653.134399999995</v>
+      </c>
+      <c r="C5" s="6">
+        <f>AVERAGE(1526.96,1321.721,1386.113,1389.112,1353.769)</f>
+        <v>1395.5350000000001</v>
+      </c>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="B6" s="8">
+        <f>AVERAGE(35636.852,35637.719,35636.688,35636.359,35636.359)</f>
+        <v>35636.795399999995</v>
+      </c>
+      <c r="C6" s="6">
+        <f>AVERAGE(1629.9,1513.463,1684.096,1323.911,1351.28)</f>
+        <v>1500.5300000000002</v>
+      </c>
+      <c r="D6" s="11">
+        <f>AVERAGE(Table1[Consumo de Datos '[kB']])</f>
+        <v>35766.054899999996</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="B4" s="6">
-        <f>B3+40</f>
-        <v>140</v>
-      </c>
-      <c r="C4" s="8">
-        <f>C3+10</f>
-        <v>85</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <f>AVERAGE(Table1[Consumo de Datos '[kB']],Table13[Consumo de Datos '[kB']])</f>
+        <v>35710.205324999995</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5" s="10">
-        <v>0.7</v>
+    <row r="9" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <f>B4+40</f>
-        <v>180</v>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
       </c>
-      <c r="C5" s="8">
-        <f>C4+10</f>
-        <v>95</v>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="12">
-        <v>0.9</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>2</v>
       </c>
-      <c r="B6" s="6">
-        <f>B5+40</f>
-        <v>220</v>
+      <c r="B11" s="9">
+        <f>AVERAGE(35696.071,35696.626,35696.376,35696.665,35695.478)</f>
+        <v>35696.243200000004</v>
       </c>
-      <c r="C6" s="8">
-        <f>C5+10</f>
-        <v>105</v>
+      <c r="C11" s="5">
+        <f>AVERAGE(1599.491,1563.487,1597.047,1549.092,1586.145)</f>
+        <v>1579.0524</v>
+      </c>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9">
+        <f>AVERAGE(35644.251,35644.376,35644.97,35644.415,35643.673)</f>
+        <v>35644.337</v>
+      </c>
+      <c r="C12" s="8">
+        <f>AVERAGE(1686.253,1409.068,1637.324,1600.361,1606.661)</f>
+        <v>1587.9334000000001</v>
+      </c>
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9">
+        <f>AVERAGE(35640.173,35639.103,35640.235,35639.72,35639.329)</f>
+        <v>35639.712000000007</v>
+      </c>
+      <c r="C13" s="9">
+        <f>AVERAGE(1412.209,1556.134,1468.772,1685.261,1678.691)</f>
+        <v>1560.2134000000001</v>
+      </c>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>8</v>
+      </c>
+      <c r="B14" s="9">
+        <f>AVERAGE(35637.509,35637.282,35637.017,35637.118,35636.728)</f>
+        <v>35637.130799999999</v>
+      </c>
+      <c r="C14" s="8">
+        <f>AVERAGE(1438.801,1689.833,1547.204,1655.264,1671.783)</f>
+        <v>1600.577</v>
+      </c>
+      <c r="D14" s="11">
+        <f>AVERAGE(Table13[Consumo de Datos '[kB']])</f>
+        <v>35654.355750000002</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.5">
-      <c r="A9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>100</v>
-      </c>
-      <c r="C11" s="5">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" s="2">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2">
-        <f>B11+30</f>
-        <v>130</v>
-      </c>
-      <c r="C12" s="6">
-        <f>C11+20</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A13" s="2">
-        <v>6</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A14" s="2">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2">
-        <f>B12+30</f>
-        <v>160</v>
-      </c>
-      <c r="C14" s="6">
-        <f>C12+20</f>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="23" ht="14.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>

</xml_diff>